<commit_message>
add minor data computation
</commit_message>
<xml_diff>
--- a/real_robot_data_plots_and_demos/orientation_experiments/valve_turn_case_1/act_tf_and_joint_states_data_euler.xlsx
+++ b/real_robot_data_plots_and_demos/orientation_experiments/valve_turn_case_1/act_tf_and_joint_states_data_euler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janak\Documents\GitHub\closed_chain_affordance\real_robot_data_plots_and_demos\orientation_experiments\fix_in_world\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janak\Documents\GitHub\closed_chain_affordance\real_robot_data_plots_and_demos\orientation_experiments\valve_turn_case_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BA20F4AE-2258-41D1-99AA-8CBA3DE44910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240F1643-2F57-4242-9CBE-61849F6246D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="act_tf_and_joint_states_data" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>arm0_shoulder_yaw</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>max of all</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,6 +449,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,10 +619,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1142,6 +1155,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-0.10814412499999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2288,7 +2304,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,9 +3123,26 @@
         <v>-6.0818319999999954E-3</v>
       </c>
     </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="4" cm="1">
+        <f t="array" ref="S13">MAX(ABS(S3:S12))</f>
+        <v>1.4473950999999818E-2</v>
+      </c>
+      <c r="T13" s="4" cm="1">
+        <f t="array" ref="T13">MAX(ABS(T3:T12))</f>
+        <v>0.11480143</v>
+      </c>
+      <c r="U13" s="4" cm="1">
+        <f t="array" ref="U13">MAX(ABS(U3:U12))</f>
+        <v>1.0089926999999999E-2</v>
+      </c>
+    </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T14" s="2" cm="1">
         <f t="array" ref="T14">MAX(ABS(S3:U12))</f>
@@ -3118,6 +3151,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>